<commit_message>
small edit to dictionary and cleaned charts
</commit_message>
<xml_diff>
--- a/scifi_syndic_conceptdic.xlsx
+++ b/scifi_syndic_conceptdic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlberlow/GitHub/SciFi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B068FBA-4CBE-A742-ACE5-E0889F43703D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81FEA4C-CC51-A14C-AF7C-9EB37D1CB2A9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{33A432A2-A9BF-3145-9568-9BCFEC5AE131}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{33A432A2-A9BF-3145-9568-9BCFEC5AE131}"/>
   </bookViews>
   <sheets>
     <sheet name="search-keyword dict" sheetId="1" r:id="rId1"/>
@@ -2943,7 +2943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C35ECC-9940-5943-BB7B-02DC105EDB3E}">
   <dimension ref="A1:XFC695"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A663" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -25474,9 +25474,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E1E5593-8547-B540-A1B9-954B51E495F5}">
   <dimension ref="A1:D170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -25498,42 +25498,42 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="17" t="s">
-        <v>774</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>758</v>
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>801</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="17" t="s">
+        <v>779</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>780</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>780</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>781</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="17" t="s">
-        <v>779</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>780</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>760</v>
       </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="10" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>780</v>
@@ -25544,20 +25544,20 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>780</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="17" t="s">
+        <v>783</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>780</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -25566,32 +25566,32 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="17" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>780</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="17" t="s">
-        <v>782</v>
-      </c>
-      <c r="B9" s="17" t="s">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>780</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="10" t="s">
-        <v>45</v>
+        <v>296</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>760</v>
@@ -25599,54 +25599,54 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="10" t="s">
-        <v>40</v>
+        <v>286</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>788</v>
+        <v>780</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="10" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>789</v>
+        <v>780</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>789</v>
+      <c r="A13" s="17" t="s">
+        <v>785</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>780</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>784</v>
+        <v>759</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>788</v>
+      <c r="A14" s="17" t="s">
+        <v>486</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>780</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>794</v>
+      <c r="A15" s="17" t="s">
+        <v>787</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>780</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>760</v>
@@ -25654,31 +25654,31 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>800</v>
+        <v>780</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>780</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>760</v>
+        <v>784</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="17" t="s">
+        <v>786</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>780</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -25687,32 +25687,32 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="10" t="s">
-        <v>338</v>
+        <v>109</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>791</v>
+        <v>780</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>784</v>
+        <v>760</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="10" t="s">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>800</v>
+        <v>788</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="10" t="s">
-        <v>101</v>
+        <v>40</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>758</v>
+        <v>788</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>760</v>
@@ -25720,10 +25720,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>802</v>
+        <v>788</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>760</v>
@@ -25731,10 +25731,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="10" t="s">
-        <v>104</v>
+        <v>35</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>797</v>
+        <v>788</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>781</v>
@@ -25742,10 +25742,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="10" t="s">
-        <v>261</v>
+        <v>50</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>760</v>
@@ -25753,384 +25753,384 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="10" t="s">
-        <v>146</v>
+        <v>37</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>802</v>
+        <v>788</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="17" t="s">
-        <v>772</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>758</v>
+      <c r="A26" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>788</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>790</v>
+        <v>634</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>788</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="10" t="s">
-        <v>191</v>
+        <v>686</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="17" t="s">
-        <v>770</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>758</v>
+      <c r="A29" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>788</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>759</v>
+        <v>784</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="10" t="s">
-        <v>169</v>
+        <v>56</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>796</v>
+        <v>789</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>760</v>
+        <v>784</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="10" t="s">
-        <v>213</v>
+        <v>57</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>760</v>
+        <v>784</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="10" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="10" t="s">
-        <v>457</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>791</v>
+      <c r="A33" s="17" t="s">
+        <v>774</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>784</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="17" t="s">
-        <v>773</v>
-      </c>
-      <c r="B34" s="17" t="s">
+      <c r="A34" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>758</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>784</v>
+        <v>760</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>794</v>
+      <c r="A35" s="17" t="s">
+        <v>772</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>792</v>
+      <c r="A36" s="17" t="s">
+        <v>770</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C36" s="10" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="17" t="s">
+        <v>773</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="17" t="s">
+        <v>776</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="17" t="s">
+        <v>778</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="17" t="s">
+        <v>775</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="17" t="s">
+        <v>767</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>760</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="10" t="s">
-        <v>652</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>797</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>792</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>796</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>790</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>800</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>790</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>790</v>
+        <v>355</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>758</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="10" t="s">
-        <v>262</v>
+        <v>206</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>798</v>
+        <v>758</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="45" spans="1:3">
-      <c r="A45" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>800</v>
+      <c r="A45" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="10" t="s">
-        <v>268</v>
+        <v>150</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>800</v>
+        <v>758</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="17" t="s">
-        <v>776</v>
+        <v>768</v>
       </c>
       <c r="B47" s="17" t="s">
         <v>758</v>
       </c>
       <c r="C47" s="10" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>758</v>
+      </c>
+      <c r="C48" s="10" t="s">
         <v>759</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="17" t="s">
-        <v>778</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>758</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="10" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>788</v>
+        <v>758</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="10" t="s">
-        <v>178</v>
+      <c r="A50" s="17" t="s">
+        <v>764</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>797</v>
+        <v>758</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="17" t="s">
-        <v>775</v>
-      </c>
-      <c r="B51" s="17" t="s">
+      <c r="A51" s="10" t="s">
+        <v>531</v>
+      </c>
+      <c r="B51" s="10" t="s">
         <v>758</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>784</v>
+        <v>759</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="17" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
       <c r="B52" s="17" t="s">
         <v>758</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>784</v>
+        <v>759</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="10" t="s">
-        <v>300</v>
+        <v>529</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>795</v>
+        <v>758</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>792</v>
+      <c r="A54" s="17" t="s">
+        <v>771</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C54" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>788</v>
+      <c r="A55" s="17" t="s">
+        <v>763</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="A56" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>788</v>
+      <c r="A56" s="17" t="s">
+        <v>769</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C56" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>800</v>
+      <c r="A57" s="17" t="s">
+        <v>777</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="58" spans="1:3">
-      <c r="A58" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>780</v>
+      <c r="A58" s="17" t="s">
+        <v>567</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="59" spans="1:3">
-      <c r="A59" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>800</v>
+      <c r="A59" s="17" t="s">
+        <v>590</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>758</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>760</v>
@@ -26138,10 +26138,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>797</v>
+        <v>159</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>758</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>760</v>
@@ -26149,29 +26149,29 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="10" t="s">
-        <v>165</v>
+        <v>106</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>792</v>
+        <v>758</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="17" t="s">
-        <v>350</v>
-      </c>
-      <c r="B62" s="17" t="s">
+      <c r="A62" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="B62" s="10" t="s">
         <v>758</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="10" t="s">
-        <v>355</v>
+        <v>144</v>
       </c>
       <c r="B63" s="10" t="s">
         <v>758</v>
@@ -26181,10 +26181,10 @@
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="B64" s="10" t="s">
+      <c r="A64" s="17" t="s">
+        <v>766</v>
+      </c>
+      <c r="B64" s="17" t="s">
         <v>758</v>
       </c>
       <c r="C64" s="10" t="s">
@@ -26192,44 +26192,44 @@
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="10" t="s">
-        <v>374</v>
+      <c r="A65" s="17" t="s">
+        <v>765</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>800</v>
+        <v>758</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>792</v>
+        <v>407</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>758</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>792</v>
+        <v>65</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>802</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="10" t="s">
-        <v>367</v>
+        <v>146</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>796</v>
+        <v>802</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>760</v>
@@ -26237,21 +26237,21 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="10" t="s">
-        <v>273</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>796</v>
+        <v>261</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>790</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>780</v>
+        <v>187</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>790</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>781</v>
@@ -26259,54 +26259,54 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>792</v>
+        <v>222</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>790</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="17" t="s">
-        <v>412</v>
+      <c r="A72" s="10" t="s">
+        <v>257</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>758</v>
+        <v>790</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>792</v>
+        <v>255</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>790</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="10" t="s">
-        <v>417</v>
-      </c>
-      <c r="B74" s="17" t="s">
-        <v>792</v>
+        <v>189</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>790</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="10" t="s">
-        <v>303</v>
+        <v>139</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C75" s="10" t="s">
         <v>760</v>
@@ -26314,54 +26314,54 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="10" t="s">
-        <v>150</v>
+        <v>6</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>758</v>
+        <v>790</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="17" t="s">
-        <v>768</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>758</v>
+      <c r="A77" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>790</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>784</v>
+        <v>760</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="10" t="s">
-        <v>121</v>
+        <v>338</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>758</v>
+        <v>791</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>759</v>
+        <v>784</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="17" t="s">
-        <v>785</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>780</v>
+      <c r="A79" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>791</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>759</v>
+        <v>784</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="10" t="s">
-        <v>565</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>797</v>
+        <v>303</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>791</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>760</v>
@@ -26380,87 +26380,87 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="10" t="s">
-        <v>452</v>
+        <v>58</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="10" t="s">
-        <v>333</v>
+        <v>466</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B84" s="10" t="s">
-        <v>792</v>
+        <v>321</v>
+      </c>
+      <c r="B84" s="17" t="s">
+        <v>791</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>788</v>
+        <v>60</v>
+      </c>
+      <c r="B85" s="17" t="s">
+        <v>791</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>797</v>
+        <v>312</v>
+      </c>
+      <c r="B86" s="17" t="s">
+        <v>791</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>760</v>
+        <v>784</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="10" t="s">
-        <v>83</v>
+        <v>191</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>758</v>
+        <v>792</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="10" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="A89" s="17" t="s">
-        <v>486</v>
-      </c>
-      <c r="B89" s="17" t="s">
-        <v>780</v>
+      <c r="A89" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>792</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>760</v>
@@ -26468,29 +26468,29 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="10" t="s">
-        <v>280</v>
+        <v>233</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="B91" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="10" t="s">
         <v>792</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="10" t="s">
-        <v>501</v>
+        <v>227</v>
       </c>
       <c r="B92" s="10" t="s">
         <v>792</v>
@@ -26501,32 +26501,32 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="10" t="s">
-        <v>704</v>
+        <v>165</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="94" spans="1:3">
-      <c r="A94" s="17" t="s">
-        <v>787</v>
+      <c r="A94" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>780</v>
+        <v>792</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" s="17" t="s">
-        <v>764</v>
+      <c r="A95" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>758</v>
+        <v>792</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>759</v>
@@ -26534,62 +26534,62 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>801</v>
+        <v>201</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>792</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="10" t="s">
-        <v>175</v>
+        <v>47</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="10" t="s">
-        <v>172</v>
+        <v>417</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="10" t="s">
-        <v>531</v>
+        <v>43</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>758</v>
+        <v>792</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B100" s="10" t="s">
-        <v>791</v>
+        <v>372</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>792</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="10" t="s">
-        <v>540</v>
+        <v>501</v>
       </c>
       <c r="B101" s="10" t="s">
         <v>792</v>
@@ -26600,98 +26600,98 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="10" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B102" s="10" t="s">
         <v>792</v>
       </c>
       <c r="C102" s="10" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="B103" s="10" t="s">
+        <v>792</v>
+      </c>
+      <c r="C103" s="10" t="s">
         <v>781</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="17" t="s">
-        <v>761</v>
-      </c>
-      <c r="B103" s="17" t="s">
-        <v>758</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>759</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="10" t="s">
-        <v>529</v>
+        <v>259</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>758</v>
+        <v>792</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="10" t="s">
-        <v>236</v>
+        <v>344</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="C105" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="17" t="s">
-        <v>771</v>
+      <c r="A106" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>758</v>
+        <v>792</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="17" t="s">
-        <v>763</v>
-      </c>
-      <c r="B107" s="17" t="s">
-        <v>758</v>
+      <c r="A107" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B107" s="10" t="s">
+        <v>792</v>
       </c>
       <c r="C107" s="10" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>792</v>
+      </c>
+      <c r="C108" s="10" t="s">
         <v>759</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="17" t="s">
-        <v>769</v>
-      </c>
-      <c r="B108" s="17" t="s">
-        <v>758</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>760</v>
-      </c>
-    </row>
     <row r="109" spans="1:3">
-      <c r="A109" s="17" t="s">
-        <v>777</v>
-      </c>
-      <c r="B109" s="17" t="s">
-        <v>758</v>
+      <c r="A109" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>797</v>
       </c>
       <c r="C109" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="B110" s="17" t="s">
-        <v>796</v>
+        <v>652</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>797</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>781</v>
@@ -26699,76 +26699,76 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B111" s="10" t="s">
-        <v>780</v>
+        <v>178</v>
+      </c>
+      <c r="B111" s="17" t="s">
+        <v>797</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="10" t="s">
-        <v>558</v>
-      </c>
-      <c r="B112" s="10" t="s">
-        <v>798</v>
+        <v>181</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>797</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="10" t="s">
-        <v>116</v>
+        <v>565</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>801</v>
+        <v>797</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="114" spans="1:3">
-      <c r="A114" s="17" t="s">
-        <v>567</v>
-      </c>
-      <c r="B114" s="17" t="s">
-        <v>758</v>
+      <c r="A114" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B114" s="10" t="s">
+        <v>797</v>
       </c>
       <c r="C114" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="B115" s="17" t="s">
-        <v>799</v>
+        <v>71</v>
+      </c>
+      <c r="B115" s="10" t="s">
+        <v>794</v>
       </c>
       <c r="C115" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="10" t="s">
-        <v>243</v>
+        <v>135</v>
       </c>
       <c r="B116" s="10" t="s">
-        <v>800</v>
+        <v>794</v>
       </c>
       <c r="C116" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="10" t="s">
-        <v>62</v>
+        <v>300</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>789</v>
+        <v>795</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>760</v>
@@ -26776,10 +26776,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="10" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="B118" s="10" t="s">
-        <v>790</v>
+        <v>796</v>
       </c>
       <c r="C118" s="10" t="s">
         <v>760</v>
@@ -26787,75 +26787,75 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="10" t="s">
-        <v>6</v>
+        <v>245</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>790</v>
+        <v>796</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="10" t="s">
-        <v>587</v>
+        <v>367</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="121" spans="1:3">
-      <c r="A121" s="17" t="s">
-        <v>590</v>
+      <c r="A121" s="10" t="s">
+        <v>273</v>
       </c>
       <c r="B121" s="17" t="s">
-        <v>758</v>
+        <v>796</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="10" t="s">
-        <v>159</v>
+        <v>280</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>758</v>
+        <v>796</v>
       </c>
       <c r="C122" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="10" t="s">
-        <v>259</v>
+        <v>704</v>
       </c>
       <c r="B123" s="10" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="C123" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="10" t="s">
-        <v>106</v>
+        <v>175</v>
       </c>
       <c r="B124" s="10" t="s">
-        <v>758</v>
+        <v>796</v>
       </c>
       <c r="C124" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B125" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B125" s="17" t="s">
         <v>796</v>
       </c>
       <c r="C125" s="10" t="s">
@@ -26864,10 +26864,10 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="10" t="s">
-        <v>472</v>
+        <v>236</v>
       </c>
       <c r="B126" s="10" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="C126" s="10" t="s">
         <v>781</v>
@@ -26875,29 +26875,29 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="B127" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B127" s="17" t="s">
         <v>796</v>
       </c>
       <c r="C127" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="10" t="s">
-        <v>351</v>
+        <v>137</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>758</v>
+        <v>796</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="10" t="s">
-        <v>211</v>
+        <v>403</v>
       </c>
       <c r="B129" s="10" t="s">
         <v>796</v>
@@ -26908,54 +26908,54 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="10" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
       <c r="B130" s="10" t="s">
-        <v>758</v>
+        <v>796</v>
       </c>
       <c r="C130" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="131" spans="1:3">
-      <c r="A131" s="17" t="s">
-        <v>766</v>
-      </c>
-      <c r="B131" s="17" t="s">
-        <v>758</v>
+      <c r="A131" s="10" t="s">
+        <v>625</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>796</v>
       </c>
       <c r="C131" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="10" t="s">
-        <v>625</v>
+        <v>87</v>
       </c>
       <c r="B132" s="10" t="s">
         <v>796</v>
       </c>
       <c r="C132" s="10" t="s">
-        <v>781</v>
+        <v>760</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="10" t="s">
-        <v>12</v>
+        <v>658</v>
       </c>
       <c r="B133" s="10" t="s">
-        <v>780</v>
+        <v>796</v>
       </c>
       <c r="C133" s="10" t="s">
-        <v>784</v>
+        <v>760</v>
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="A134" s="17" t="s">
-        <v>786</v>
-      </c>
-      <c r="B134" s="17" t="s">
-        <v>780</v>
+      <c r="A134" s="10" t="s">
+        <v>525</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>796</v>
       </c>
       <c r="C134" s="10" t="s">
         <v>760</v>
@@ -26963,21 +26963,21 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="10" t="s">
-        <v>344</v>
+        <v>54</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>792</v>
+        <v>796</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="10" t="s">
-        <v>634</v>
-      </c>
-      <c r="B136" s="10" t="s">
-        <v>788</v>
+        <v>111</v>
+      </c>
+      <c r="B136" s="17" t="s">
+        <v>796</v>
       </c>
       <c r="C136" s="10" t="s">
         <v>760</v>
@@ -26985,10 +26985,10 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="10" t="s">
-        <v>87</v>
+        <v>340</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C137" s="10" t="s">
         <v>760</v>
@@ -26996,40 +26996,40 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="10" t="s">
-        <v>658</v>
+        <v>262</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="10" t="s">
-        <v>109</v>
+        <v>558</v>
       </c>
       <c r="B139" s="10" t="s">
-        <v>780</v>
+        <v>798</v>
       </c>
       <c r="C139" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="10" t="s">
-        <v>644</v>
+        <v>587</v>
       </c>
       <c r="B140" s="10" t="s">
         <v>798</v>
       </c>
       <c r="C140" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="10" t="s">
-        <v>292</v>
+        <v>644</v>
       </c>
       <c r="B141" s="10" t="s">
         <v>798</v>
@@ -27040,21 +27040,21 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="10" t="s">
-        <v>330</v>
+        <v>292</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="10" t="s">
-        <v>75</v>
+        <v>250</v>
       </c>
       <c r="B143" s="17" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C143" s="10" t="s">
         <v>760</v>
@@ -27062,31 +27062,31 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="10" t="s">
-        <v>463</v>
-      </c>
-      <c r="B144" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="B144" s="17" t="s">
         <v>799</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="10" t="s">
-        <v>454</v>
+        <v>330</v>
       </c>
       <c r="B145" s="10" t="s">
         <v>799</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>781</v>
+        <v>759</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B146" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B146" s="17" t="s">
         <v>799</v>
       </c>
       <c r="C146" s="10" t="s">
@@ -27095,32 +27095,32 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="B147" s="17" t="s">
-        <v>798</v>
+        <v>463</v>
+      </c>
+      <c r="B147" s="10" t="s">
+        <v>799</v>
       </c>
       <c r="C147" s="10" t="s">
         <v>760</v>
       </c>
     </row>
     <row r="148" spans="1:3">
-      <c r="A148" s="17" t="s">
-        <v>765</v>
-      </c>
-      <c r="B148" s="17" t="s">
-        <v>758</v>
+      <c r="A148" s="10" t="s">
+        <v>454</v>
+      </c>
+      <c r="B148" s="10" t="s">
+        <v>799</v>
       </c>
       <c r="C148" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B149" s="17" t="s">
-        <v>792</v>
+        <v>128</v>
+      </c>
+      <c r="B149" s="10" t="s">
+        <v>799</v>
       </c>
       <c r="C149" s="10" t="s">
         <v>760</v>
@@ -27128,76 +27128,76 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="10" t="s">
-        <v>407</v>
+        <v>84</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>758</v>
+        <v>800</v>
       </c>
       <c r="C150" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="10" t="s">
-        <v>686</v>
+        <v>113</v>
       </c>
       <c r="B151" s="10" t="s">
-        <v>788</v>
+        <v>800</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="10" t="s">
-        <v>525</v>
+        <v>248</v>
       </c>
       <c r="B152" s="10" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="B153" s="17" t="s">
-        <v>791</v>
+        <v>263</v>
+      </c>
+      <c r="B153" s="10" t="s">
+        <v>800</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="10" t="s">
-        <v>152</v>
+        <v>268</v>
       </c>
       <c r="B154" s="10" t="s">
-        <v>790</v>
+        <v>800</v>
       </c>
       <c r="C154" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="B155" s="17" t="s">
-        <v>791</v>
+        <v>319</v>
+      </c>
+      <c r="B155" s="10" t="s">
+        <v>800</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B156" s="17" t="s">
-        <v>791</v>
+        <v>325</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>800</v>
       </c>
       <c r="C156" s="10" t="s">
         <v>760</v>
@@ -27205,87 +27205,87 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="B157" s="10" t="s">
-        <v>792</v>
+        <v>374</v>
+      </c>
+      <c r="B157" s="17" t="s">
+        <v>800</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="10" t="s">
-        <v>54</v>
+        <v>243</v>
       </c>
       <c r="B158" s="10" t="s">
-        <v>796</v>
+        <v>800</v>
       </c>
       <c r="C158" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="10" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B159" s="17" t="s">
-        <v>792</v>
+        <v>800</v>
       </c>
       <c r="C159" s="10" t="s">
-        <v>759</v>
+        <v>781</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B160" s="17" t="s">
-        <v>796</v>
+        <v>452</v>
+      </c>
+      <c r="B160" s="10" t="s">
+        <v>801</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="10" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="B161" s="17" t="s">
-        <v>791</v>
+        <v>801</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="B162" s="10" t="s">
-        <v>793</v>
+        <v>132</v>
+      </c>
+      <c r="B162" s="17" t="s">
+        <v>801</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="B163" s="10" t="s">
-        <v>788</v>
+        <v>116</v>
+      </c>
+      <c r="B163" s="17" t="s">
+        <v>801</v>
       </c>
       <c r="C163" s="10" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B164" s="17" t="s">
-        <v>800</v>
+        <v>472</v>
+      </c>
+      <c r="B164" s="10" t="s">
+        <v>801</v>
       </c>
       <c r="C164" s="10" t="s">
         <v>781</v>
@@ -27313,7 +27313,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:C170">
-    <sortCondition ref="A1"/>
+    <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>